<commit_message>
Refactoring preflight.py changes through 8/26/24 17:00
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E943FFC9-5015-4754-A3C6-1231E72C893E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828664BE-BAC6-4944-89DB-B610A4646DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1087" yWindow="1455" windowWidth="28801" windowHeight="11588" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="19440" windowHeight="11858" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>